<commit_message>
Return sheet/cell in warning of impossible date
</commit_message>
<xml_diff>
--- a/tests/testthat/1900-02-29.xlsx
+++ b/tests/testthat/1900-02-29.xlsx
@@ -350,11 +350,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -362,6 +360,9 @@
       <c r="A1" s="1">
         <v>60</v>
       </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>